<commit_message>
Added MODALIDAD to district level info
</commit_message>
<xml_diff>
--- a/_FUZZY-at-local-LISTO.xlsx
+++ b/_FUZZY-at-local-LISTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\egtpi-gs-at\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9331B6EC-D7B7-48E1-830A-E4228AC05D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80903D0-EEEA-4DE8-88AD-9044F976102F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$921</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$989</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7375" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8038" uniqueCount="1290">
   <si>
     <t>UBIGEO</t>
   </si>
@@ -3770,6 +3770,129 @@
   </si>
   <si>
     <t>160113</t>
+  </si>
+  <si>
+    <t>030702</t>
+  </si>
+  <si>
+    <t>CURPAHUASI</t>
+  </si>
+  <si>
+    <t>030304</t>
+  </si>
+  <si>
+    <t>ANTABAMBA</t>
+  </si>
+  <si>
+    <t>JUAN ESPINOZA MEDRANO</t>
+  </si>
+  <si>
+    <t>080805</t>
+  </si>
+  <si>
+    <t>ESPINAR</t>
+  </si>
+  <si>
+    <t>PALLPATA</t>
+  </si>
+  <si>
+    <t>080506</t>
+  </si>
+  <si>
+    <t>080504</t>
+  </si>
+  <si>
+    <t>LANGUI</t>
+  </si>
+  <si>
+    <t>080808</t>
+  </si>
+  <si>
+    <t>ALTO PICHIGUA</t>
+  </si>
+  <si>
+    <t>080806</t>
+  </si>
+  <si>
+    <t>PICHIGUA</t>
+  </si>
+  <si>
+    <t>080807</t>
+  </si>
+  <si>
+    <t>SUYCKUTAMBO</t>
+  </si>
+  <si>
+    <t>SUYKUTAMBO</t>
+  </si>
+  <si>
+    <t>080804</t>
+  </si>
+  <si>
+    <t>OCORURO</t>
+  </si>
+  <si>
+    <t>080801</t>
+  </si>
+  <si>
+    <t>220808</t>
+  </si>
+  <si>
+    <t>YORONGOS</t>
+  </si>
+  <si>
+    <t>220913</t>
+  </si>
+  <si>
+    <t>SAUCE</t>
+  </si>
+  <si>
+    <t>220703</t>
+  </si>
+  <si>
+    <t>CASPISAPA</t>
+  </si>
+  <si>
+    <t>051006</t>
+  </si>
+  <si>
+    <t>CAYARA</t>
+  </si>
+  <si>
+    <t>051012</t>
+  </si>
+  <si>
+    <t>VILCANCHOS</t>
+  </si>
+  <si>
+    <t>051108</t>
+  </si>
+  <si>
+    <t>VISCHONGO</t>
+  </si>
+  <si>
+    <t>FAJARDO</t>
+  </si>
+  <si>
+    <t>110207</t>
+  </si>
+  <si>
+    <t>220402</t>
+  </si>
+  <si>
+    <t>ALTO SAPOSOA</t>
+  </si>
+  <si>
+    <t>081304</t>
+  </si>
+  <si>
+    <t>MACHUPICCHU</t>
+  </si>
+  <si>
+    <t>220908</t>
+  </si>
+  <si>
+    <t>JUAN GUERRA</t>
   </si>
 </sst>
 </file>
@@ -4157,10 +4280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M924"/>
+  <dimension ref="A1:M1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A907" workbookViewId="0">
-      <selection activeCell="M922" sqref="M922:M924"/>
+    <sheetView tabSelected="1" topLeftCell="A984" workbookViewId="0">
+      <selection activeCell="M1008" sqref="M1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42052,8 +42175,3411 @@
         <v>932</v>
       </c>
     </row>
+    <row r="925" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B925" t="s">
+        <v>109</v>
+      </c>
+      <c r="C925" t="s">
+        <v>155</v>
+      </c>
+      <c r="D925" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E925" t="s">
+        <v>109</v>
+      </c>
+      <c r="F925" t="s">
+        <v>155</v>
+      </c>
+      <c r="G925" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H925">
+        <v>1343</v>
+      </c>
+      <c r="I925">
+        <v>0</v>
+      </c>
+      <c r="J925">
+        <v>0</v>
+      </c>
+      <c r="K925">
+        <v>0</v>
+      </c>
+      <c r="L925">
+        <v>0</v>
+      </c>
+      <c r="M925" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="926" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
+        <v>592</v>
+      </c>
+      <c r="B926" t="s">
+        <v>585</v>
+      </c>
+      <c r="C926" t="s">
+        <v>586</v>
+      </c>
+      <c r="D926" t="s">
+        <v>593</v>
+      </c>
+      <c r="E926" t="s">
+        <v>585</v>
+      </c>
+      <c r="F926" t="s">
+        <v>586</v>
+      </c>
+      <c r="G926" t="s">
+        <v>593</v>
+      </c>
+      <c r="H926">
+        <v>1346</v>
+      </c>
+      <c r="I926">
+        <v>0</v>
+      </c>
+      <c r="J926">
+        <v>0</v>
+      </c>
+      <c r="K926">
+        <v>0</v>
+      </c>
+      <c r="L926">
+        <v>0</v>
+      </c>
+      <c r="M926" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="927" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B927" t="s">
+        <v>317</v>
+      </c>
+      <c r="C927" t="s">
+        <v>708</v>
+      </c>
+      <c r="D927" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E927" t="s">
+        <v>317</v>
+      </c>
+      <c r="F927" t="s">
+        <v>708</v>
+      </c>
+      <c r="G927" t="s">
+        <v>1096</v>
+      </c>
+      <c r="H927">
+        <v>1347</v>
+      </c>
+      <c r="I927">
+        <v>0</v>
+      </c>
+      <c r="J927">
+        <v>0</v>
+      </c>
+      <c r="K927">
+        <v>0</v>
+      </c>
+      <c r="L927">
+        <v>0</v>
+      </c>
+      <c r="M927" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="928" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B928" t="s">
+        <v>109</v>
+      </c>
+      <c r="C928" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D928" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E928" t="s">
+        <v>109</v>
+      </c>
+      <c r="F928" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G928" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H928">
+        <v>1348</v>
+      </c>
+      <c r="I928">
+        <v>0</v>
+      </c>
+      <c r="J928">
+        <v>0</v>
+      </c>
+      <c r="K928">
+        <v>0</v>
+      </c>
+      <c r="L928">
+        <v>0</v>
+      </c>
+      <c r="M928" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="929" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>387</v>
+      </c>
+      <c r="B929" t="s">
+        <v>346</v>
+      </c>
+      <c r="C929" t="s">
+        <v>346</v>
+      </c>
+      <c r="D929" t="s">
+        <v>388</v>
+      </c>
+      <c r="E929" t="s">
+        <v>346</v>
+      </c>
+      <c r="F929" t="s">
+        <v>346</v>
+      </c>
+      <c r="G929" t="s">
+        <v>388</v>
+      </c>
+      <c r="H929">
+        <v>1350</v>
+      </c>
+      <c r="I929">
+        <v>0</v>
+      </c>
+      <c r="J929">
+        <v>0</v>
+      </c>
+      <c r="K929">
+        <v>0</v>
+      </c>
+      <c r="L929">
+        <v>0</v>
+      </c>
+      <c r="M929" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="930" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>622</v>
+      </c>
+      <c r="B930" t="s">
+        <v>585</v>
+      </c>
+      <c r="C930" t="s">
+        <v>585</v>
+      </c>
+      <c r="D930" t="s">
+        <v>585</v>
+      </c>
+      <c r="E930" t="s">
+        <v>585</v>
+      </c>
+      <c r="F930" t="s">
+        <v>585</v>
+      </c>
+      <c r="G930" t="s">
+        <v>585</v>
+      </c>
+      <c r="H930">
+        <v>1351</v>
+      </c>
+      <c r="I930">
+        <v>0</v>
+      </c>
+      <c r="J930">
+        <v>0</v>
+      </c>
+      <c r="K930">
+        <v>0</v>
+      </c>
+      <c r="L930">
+        <v>0</v>
+      </c>
+      <c r="M930" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="931" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A931" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B931" t="s">
+        <v>317</v>
+      </c>
+      <c r="C931" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D931" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E931" t="s">
+        <v>317</v>
+      </c>
+      <c r="F931" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G931" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H931">
+        <v>1353</v>
+      </c>
+      <c r="I931">
+        <v>0</v>
+      </c>
+      <c r="J931">
+        <v>0</v>
+      </c>
+      <c r="K931">
+        <v>0</v>
+      </c>
+      <c r="L931">
+        <v>0</v>
+      </c>
+      <c r="M931" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="932" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A932" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B932" t="s">
+        <v>317</v>
+      </c>
+      <c r="C932" t="s">
+        <v>321</v>
+      </c>
+      <c r="D932" t="s">
+        <v>473</v>
+      </c>
+      <c r="E932" t="s">
+        <v>317</v>
+      </c>
+      <c r="F932" t="s">
+        <v>321</v>
+      </c>
+      <c r="G932" t="s">
+        <v>473</v>
+      </c>
+      <c r="H932">
+        <v>1354</v>
+      </c>
+      <c r="I932">
+        <v>0</v>
+      </c>
+      <c r="J932">
+        <v>0</v>
+      </c>
+      <c r="K932">
+        <v>0</v>
+      </c>
+      <c r="L932">
+        <v>0</v>
+      </c>
+      <c r="M932" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="933" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B933" t="s">
+        <v>317</v>
+      </c>
+      <c r="C933" t="s">
+        <v>321</v>
+      </c>
+      <c r="D933" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E933" t="s">
+        <v>317</v>
+      </c>
+      <c r="F933" t="s">
+        <v>321</v>
+      </c>
+      <c r="G933" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H933">
+        <v>1355</v>
+      </c>
+      <c r="I933">
+        <v>0</v>
+      </c>
+      <c r="J933">
+        <v>0</v>
+      </c>
+      <c r="K933">
+        <v>0</v>
+      </c>
+      <c r="L933">
+        <v>0</v>
+      </c>
+      <c r="M933" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="934" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A934" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B934" t="s">
+        <v>317</v>
+      </c>
+      <c r="C934" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D934" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E934" t="s">
+        <v>317</v>
+      </c>
+      <c r="F934" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G934" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H934">
+        <v>1356</v>
+      </c>
+      <c r="I934">
+        <v>0</v>
+      </c>
+      <c r="J934">
+        <v>0</v>
+      </c>
+      <c r="K934">
+        <v>0</v>
+      </c>
+      <c r="L934">
+        <v>0</v>
+      </c>
+      <c r="M934" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="935" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A935" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B935" t="s">
+        <v>317</v>
+      </c>
+      <c r="C935" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D935" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E935" t="s">
+        <v>317</v>
+      </c>
+      <c r="F935" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G935" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H935">
+        <v>1357</v>
+      </c>
+      <c r="I935">
+        <v>0</v>
+      </c>
+      <c r="J935">
+        <v>0</v>
+      </c>
+      <c r="K935">
+        <v>0</v>
+      </c>
+      <c r="L935">
+        <v>0</v>
+      </c>
+      <c r="M935" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="936" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A936" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B936" t="s">
+        <v>317</v>
+      </c>
+      <c r="C936" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D936" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E936" t="s">
+        <v>317</v>
+      </c>
+      <c r="F936" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G936" t="s">
+        <v>1266</v>
+      </c>
+      <c r="H936">
+        <v>1360</v>
+      </c>
+      <c r="I936">
+        <v>0</v>
+      </c>
+      <c r="J936">
+        <v>0</v>
+      </c>
+      <c r="K936">
+        <v>3.030303030303028E-2</v>
+      </c>
+      <c r="L936">
+        <v>3.030303030303028E-2</v>
+      </c>
+      <c r="M936" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="937" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>323</v>
+      </c>
+      <c r="B937" t="s">
+        <v>317</v>
+      </c>
+      <c r="C937" t="s">
+        <v>321</v>
+      </c>
+      <c r="D937" t="s">
+        <v>324</v>
+      </c>
+      <c r="E937" t="s">
+        <v>317</v>
+      </c>
+      <c r="F937" t="s">
+        <v>321</v>
+      </c>
+      <c r="G937" t="s">
+        <v>324</v>
+      </c>
+      <c r="H937">
+        <v>1361</v>
+      </c>
+      <c r="I937">
+        <v>0</v>
+      </c>
+      <c r="J937">
+        <v>0</v>
+      </c>
+      <c r="K937">
+        <v>0</v>
+      </c>
+      <c r="L937">
+        <v>0</v>
+      </c>
+      <c r="M937" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="938" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>790</v>
+      </c>
+      <c r="B938" t="s">
+        <v>785</v>
+      </c>
+      <c r="C938" t="s">
+        <v>791</v>
+      </c>
+      <c r="D938" t="s">
+        <v>605</v>
+      </c>
+      <c r="E938" t="s">
+        <v>785</v>
+      </c>
+      <c r="F938" t="s">
+        <v>791</v>
+      </c>
+      <c r="G938" t="s">
+        <v>605</v>
+      </c>
+      <c r="H938">
+        <v>1362</v>
+      </c>
+      <c r="I938">
+        <v>0</v>
+      </c>
+      <c r="J938">
+        <v>0</v>
+      </c>
+      <c r="K938">
+        <v>0</v>
+      </c>
+      <c r="L938">
+        <v>0</v>
+      </c>
+      <c r="M938" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="939" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B939" t="s">
+        <v>317</v>
+      </c>
+      <c r="C939" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D939" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E939" t="s">
+        <v>317</v>
+      </c>
+      <c r="F939" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G939" t="s">
+        <v>1268</v>
+      </c>
+      <c r="H939">
+        <v>1363</v>
+      </c>
+      <c r="I939">
+        <v>0</v>
+      </c>
+      <c r="J939">
+        <v>0</v>
+      </c>
+      <c r="K939">
+        <v>0</v>
+      </c>
+      <c r="L939">
+        <v>0</v>
+      </c>
+      <c r="M939" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="940" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B940" t="s">
+        <v>42</v>
+      </c>
+      <c r="C940" t="s">
+        <v>968</v>
+      </c>
+      <c r="D940" t="s">
+        <v>306</v>
+      </c>
+      <c r="E940" t="s">
+        <v>42</v>
+      </c>
+      <c r="F940" t="s">
+        <v>968</v>
+      </c>
+      <c r="G940" t="s">
+        <v>306</v>
+      </c>
+      <c r="H940">
+        <v>1366</v>
+      </c>
+      <c r="I940">
+        <v>0</v>
+      </c>
+      <c r="J940">
+        <v>0</v>
+      </c>
+      <c r="K940">
+        <v>0</v>
+      </c>
+      <c r="L940">
+        <v>0</v>
+      </c>
+      <c r="M940" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="941" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>806</v>
+      </c>
+      <c r="B941" t="s">
+        <v>785</v>
+      </c>
+      <c r="C941" t="s">
+        <v>801</v>
+      </c>
+      <c r="D941" t="s">
+        <v>807</v>
+      </c>
+      <c r="E941" t="s">
+        <v>785</v>
+      </c>
+      <c r="F941" t="s">
+        <v>801</v>
+      </c>
+      <c r="G941" t="s">
+        <v>807</v>
+      </c>
+      <c r="H941">
+        <v>1367</v>
+      </c>
+      <c r="I941">
+        <v>0</v>
+      </c>
+      <c r="J941">
+        <v>0</v>
+      </c>
+      <c r="K941">
+        <v>0</v>
+      </c>
+      <c r="L941">
+        <v>0</v>
+      </c>
+      <c r="M941" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="942" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>815</v>
+      </c>
+      <c r="B942" t="s">
+        <v>785</v>
+      </c>
+      <c r="C942" t="s">
+        <v>801</v>
+      </c>
+      <c r="D942" t="s">
+        <v>816</v>
+      </c>
+      <c r="E942" t="s">
+        <v>785</v>
+      </c>
+      <c r="F942" t="s">
+        <v>801</v>
+      </c>
+      <c r="G942" t="s">
+        <v>816</v>
+      </c>
+      <c r="H942">
+        <v>1368</v>
+      </c>
+      <c r="I942">
+        <v>0</v>
+      </c>
+      <c r="J942">
+        <v>0</v>
+      </c>
+      <c r="K942">
+        <v>0</v>
+      </c>
+      <c r="L942">
+        <v>0</v>
+      </c>
+      <c r="M942" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="943" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>845</v>
+      </c>
+      <c r="B943" t="s">
+        <v>785</v>
+      </c>
+      <c r="C943" t="s">
+        <v>838</v>
+      </c>
+      <c r="D943" t="s">
+        <v>846</v>
+      </c>
+      <c r="E943" t="s">
+        <v>785</v>
+      </c>
+      <c r="F943" t="s">
+        <v>838</v>
+      </c>
+      <c r="G943" t="s">
+        <v>846</v>
+      </c>
+      <c r="H943">
+        <v>1369</v>
+      </c>
+      <c r="I943">
+        <v>0</v>
+      </c>
+      <c r="J943">
+        <v>0</v>
+      </c>
+      <c r="K943">
+        <v>0</v>
+      </c>
+      <c r="L943">
+        <v>0</v>
+      </c>
+      <c r="M943" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="944" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A944" t="s">
+        <v>813</v>
+      </c>
+      <c r="B944" t="s">
+        <v>785</v>
+      </c>
+      <c r="C944" t="s">
+        <v>801</v>
+      </c>
+      <c r="D944" t="s">
+        <v>814</v>
+      </c>
+      <c r="E944" t="s">
+        <v>785</v>
+      </c>
+      <c r="F944" t="s">
+        <v>801</v>
+      </c>
+      <c r="G944" t="s">
+        <v>814</v>
+      </c>
+      <c r="H944">
+        <v>1370</v>
+      </c>
+      <c r="I944">
+        <v>0</v>
+      </c>
+      <c r="J944">
+        <v>0</v>
+      </c>
+      <c r="K944">
+        <v>0</v>
+      </c>
+      <c r="L944">
+        <v>0</v>
+      </c>
+      <c r="M944" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="945" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A945" t="s">
+        <v>813</v>
+      </c>
+      <c r="B945" t="s">
+        <v>785</v>
+      </c>
+      <c r="C945" t="s">
+        <v>801</v>
+      </c>
+      <c r="D945" t="s">
+        <v>814</v>
+      </c>
+      <c r="E945" t="s">
+        <v>785</v>
+      </c>
+      <c r="F945" t="s">
+        <v>801</v>
+      </c>
+      <c r="G945" t="s">
+        <v>814</v>
+      </c>
+      <c r="H945">
+        <v>1371</v>
+      </c>
+      <c r="I945">
+        <v>0</v>
+      </c>
+      <c r="J945">
+        <v>0</v>
+      </c>
+      <c r="K945">
+        <v>0</v>
+      </c>
+      <c r="L945">
+        <v>0</v>
+      </c>
+      <c r="M945" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="946" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A946" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B946" t="s">
+        <v>785</v>
+      </c>
+      <c r="C946" t="s">
+        <v>785</v>
+      </c>
+      <c r="D946" t="s">
+        <v>810</v>
+      </c>
+      <c r="E946" t="s">
+        <v>785</v>
+      </c>
+      <c r="F946" t="s">
+        <v>785</v>
+      </c>
+      <c r="G946" t="s">
+        <v>809</v>
+      </c>
+      <c r="H946">
+        <v>1374</v>
+      </c>
+      <c r="I946">
+        <v>0</v>
+      </c>
+      <c r="J946">
+        <v>0</v>
+      </c>
+      <c r="K946">
+        <v>0.2373737373737374</v>
+      </c>
+      <c r="L946">
+        <v>0.2373737373737374</v>
+      </c>
+      <c r="M946" s="2">
+        <v>220509</v>
+      </c>
+    </row>
+    <row r="947" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A947" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B947" t="s">
+        <v>317</v>
+      </c>
+      <c r="C947" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D947" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E947" t="s">
+        <v>317</v>
+      </c>
+      <c r="F947" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G947" t="s">
+        <v>1255</v>
+      </c>
+      <c r="H947">
+        <v>1375</v>
+      </c>
+      <c r="I947">
+        <v>0</v>
+      </c>
+      <c r="J947">
+        <v>0</v>
+      </c>
+      <c r="K947">
+        <v>0</v>
+      </c>
+      <c r="L947">
+        <v>0</v>
+      </c>
+      <c r="M947" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="948" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A948" t="s">
+        <v>918</v>
+      </c>
+      <c r="B948" t="s">
+        <v>913</v>
+      </c>
+      <c r="C948" t="s">
+        <v>919</v>
+      </c>
+      <c r="D948" t="s">
+        <v>920</v>
+      </c>
+      <c r="E948" t="s">
+        <v>913</v>
+      </c>
+      <c r="F948" t="s">
+        <v>919</v>
+      </c>
+      <c r="G948" t="s">
+        <v>920</v>
+      </c>
+      <c r="H948">
+        <v>1376</v>
+      </c>
+      <c r="I948">
+        <v>0</v>
+      </c>
+      <c r="J948">
+        <v>0</v>
+      </c>
+      <c r="K948">
+        <v>0</v>
+      </c>
+      <c r="L948">
+        <v>0</v>
+      </c>
+      <c r="M948" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="949" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A949" t="s">
+        <v>36</v>
+      </c>
+      <c r="B949" t="s">
+        <v>13</v>
+      </c>
+      <c r="C949" t="s">
+        <v>34</v>
+      </c>
+      <c r="D949" t="s">
+        <v>37</v>
+      </c>
+      <c r="E949" t="s">
+        <v>13</v>
+      </c>
+      <c r="F949" t="s">
+        <v>34</v>
+      </c>
+      <c r="G949" t="s">
+        <v>37</v>
+      </c>
+      <c r="H949">
+        <v>1377</v>
+      </c>
+      <c r="I949">
+        <v>0</v>
+      </c>
+      <c r="J949">
+        <v>0</v>
+      </c>
+      <c r="K949">
+        <v>0</v>
+      </c>
+      <c r="L949">
+        <v>0</v>
+      </c>
+      <c r="M949" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="950" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A950" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B950" t="s">
+        <v>785</v>
+      </c>
+      <c r="C950" t="s">
+        <v>827</v>
+      </c>
+      <c r="D950" t="s">
+        <v>827</v>
+      </c>
+      <c r="E950" t="s">
+        <v>785</v>
+      </c>
+      <c r="F950" t="s">
+        <v>827</v>
+      </c>
+      <c r="G950" t="s">
+        <v>827</v>
+      </c>
+      <c r="H950">
+        <v>1378</v>
+      </c>
+      <c r="I950">
+        <v>0</v>
+      </c>
+      <c r="J950">
+        <v>0</v>
+      </c>
+      <c r="K950">
+        <v>0</v>
+      </c>
+      <c r="L950">
+        <v>0</v>
+      </c>
+      <c r="M950" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="951" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A951" t="s">
+        <v>833</v>
+      </c>
+      <c r="B951" t="s">
+        <v>785</v>
+      </c>
+      <c r="C951" t="s">
+        <v>827</v>
+      </c>
+      <c r="D951" t="s">
+        <v>834</v>
+      </c>
+      <c r="E951" t="s">
+        <v>785</v>
+      </c>
+      <c r="F951" t="s">
+        <v>827</v>
+      </c>
+      <c r="G951" t="s">
+        <v>834</v>
+      </c>
+      <c r="H951">
+        <v>1379</v>
+      </c>
+      <c r="I951">
+        <v>0</v>
+      </c>
+      <c r="J951">
+        <v>0</v>
+      </c>
+      <c r="K951">
+        <v>0</v>
+      </c>
+      <c r="L951">
+        <v>0</v>
+      </c>
+      <c r="M951" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="952" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A952" t="s">
+        <v>829</v>
+      </c>
+      <c r="B952" t="s">
+        <v>785</v>
+      </c>
+      <c r="C952" t="s">
+        <v>827</v>
+      </c>
+      <c r="D952" t="s">
+        <v>830</v>
+      </c>
+      <c r="E952" t="s">
+        <v>785</v>
+      </c>
+      <c r="F952" t="s">
+        <v>827</v>
+      </c>
+      <c r="G952" t="s">
+        <v>830</v>
+      </c>
+      <c r="H952">
+        <v>1380</v>
+      </c>
+      <c r="I952">
+        <v>0</v>
+      </c>
+      <c r="J952">
+        <v>0</v>
+      </c>
+      <c r="K952">
+        <v>0</v>
+      </c>
+      <c r="L952">
+        <v>0</v>
+      </c>
+      <c r="M952" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="953" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>826</v>
+      </c>
+      <c r="B953" t="s">
+        <v>785</v>
+      </c>
+      <c r="C953" t="s">
+        <v>827</v>
+      </c>
+      <c r="D953" t="s">
+        <v>828</v>
+      </c>
+      <c r="E953" t="s">
+        <v>785</v>
+      </c>
+      <c r="F953" t="s">
+        <v>827</v>
+      </c>
+      <c r="G953" t="s">
+        <v>828</v>
+      </c>
+      <c r="H953">
+        <v>1381</v>
+      </c>
+      <c r="I953">
+        <v>0</v>
+      </c>
+      <c r="J953">
+        <v>0</v>
+      </c>
+      <c r="K953">
+        <v>0</v>
+      </c>
+      <c r="L953">
+        <v>0</v>
+      </c>
+      <c r="M953" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="954" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A954" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B954" t="s">
+        <v>785</v>
+      </c>
+      <c r="C954" t="s">
+        <v>785</v>
+      </c>
+      <c r="D954" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E954" t="s">
+        <v>785</v>
+      </c>
+      <c r="F954" t="s">
+        <v>785</v>
+      </c>
+      <c r="G954" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H954">
+        <v>1382</v>
+      </c>
+      <c r="I954">
+        <v>0</v>
+      </c>
+      <c r="J954">
+        <v>0</v>
+      </c>
+      <c r="K954">
+        <v>0</v>
+      </c>
+      <c r="L954">
+        <v>0</v>
+      </c>
+      <c r="M954" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="955" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A955" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B955" t="s">
+        <v>785</v>
+      </c>
+      <c r="C955" t="s">
+        <v>785</v>
+      </c>
+      <c r="D955" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E955" t="s">
+        <v>785</v>
+      </c>
+      <c r="F955" t="s">
+        <v>785</v>
+      </c>
+      <c r="G955" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H955">
+        <v>1383</v>
+      </c>
+      <c r="I955">
+        <v>0</v>
+      </c>
+      <c r="J955">
+        <v>0</v>
+      </c>
+      <c r="K955">
+        <v>0</v>
+      </c>
+      <c r="L955">
+        <v>0</v>
+      </c>
+      <c r="M955" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="956" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A956" t="s">
+        <v>848</v>
+      </c>
+      <c r="B956" t="s">
+        <v>785</v>
+      </c>
+      <c r="C956" t="s">
+        <v>849</v>
+      </c>
+      <c r="D956" t="s">
+        <v>850</v>
+      </c>
+      <c r="E956" t="s">
+        <v>785</v>
+      </c>
+      <c r="F956" t="s">
+        <v>849</v>
+      </c>
+      <c r="G956" t="s">
+        <v>850</v>
+      </c>
+      <c r="H956">
+        <v>1384</v>
+      </c>
+      <c r="I956">
+        <v>0</v>
+      </c>
+      <c r="J956">
+        <v>0</v>
+      </c>
+      <c r="K956">
+        <v>0</v>
+      </c>
+      <c r="L956">
+        <v>0</v>
+      </c>
+      <c r="M956" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="957" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A957" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B957" t="s">
+        <v>785</v>
+      </c>
+      <c r="C957" t="s">
+        <v>849</v>
+      </c>
+      <c r="D957" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E957" t="s">
+        <v>785</v>
+      </c>
+      <c r="F957" t="s">
+        <v>849</v>
+      </c>
+      <c r="G957" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H957">
+        <v>1385</v>
+      </c>
+      <c r="I957">
+        <v>0</v>
+      </c>
+      <c r="J957">
+        <v>0</v>
+      </c>
+      <c r="K957">
+        <v>0</v>
+      </c>
+      <c r="L957">
+        <v>0</v>
+      </c>
+      <c r="M957" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="958" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A958" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B958" t="s">
+        <v>785</v>
+      </c>
+      <c r="C958" t="s">
+        <v>785</v>
+      </c>
+      <c r="D958" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E958" t="s">
+        <v>785</v>
+      </c>
+      <c r="F958" t="s">
+        <v>785</v>
+      </c>
+      <c r="G958" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H958">
+        <v>1386</v>
+      </c>
+      <c r="I958">
+        <v>0</v>
+      </c>
+      <c r="J958">
+        <v>0</v>
+      </c>
+      <c r="K958">
+        <v>0</v>
+      </c>
+      <c r="L958">
+        <v>0</v>
+      </c>
+      <c r="M958" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="959" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A959" t="s">
+        <v>843</v>
+      </c>
+      <c r="B959" t="s">
+        <v>785</v>
+      </c>
+      <c r="C959" t="s">
+        <v>838</v>
+      </c>
+      <c r="D959" t="s">
+        <v>844</v>
+      </c>
+      <c r="E959" t="s">
+        <v>785</v>
+      </c>
+      <c r="F959" t="s">
+        <v>838</v>
+      </c>
+      <c r="G959" t="s">
+        <v>844</v>
+      </c>
+      <c r="H959">
+        <v>1387</v>
+      </c>
+      <c r="I959">
+        <v>0</v>
+      </c>
+      <c r="J959">
+        <v>0</v>
+      </c>
+      <c r="K959">
+        <v>0</v>
+      </c>
+      <c r="L959">
+        <v>0</v>
+      </c>
+      <c r="M959" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="960" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A960" t="s">
+        <v>840</v>
+      </c>
+      <c r="B960" t="s">
+        <v>785</v>
+      </c>
+      <c r="C960" t="s">
+        <v>838</v>
+      </c>
+      <c r="D960" t="s">
+        <v>838</v>
+      </c>
+      <c r="E960" t="s">
+        <v>785</v>
+      </c>
+      <c r="F960" t="s">
+        <v>838</v>
+      </c>
+      <c r="G960" t="s">
+        <v>838</v>
+      </c>
+      <c r="H960">
+        <v>1388</v>
+      </c>
+      <c r="I960">
+        <v>0</v>
+      </c>
+      <c r="J960">
+        <v>0</v>
+      </c>
+      <c r="K960">
+        <v>0</v>
+      </c>
+      <c r="L960">
+        <v>0</v>
+      </c>
+      <c r="M960" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="961" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A961" t="s">
+        <v>841</v>
+      </c>
+      <c r="B961" t="s">
+        <v>785</v>
+      </c>
+      <c r="C961" t="s">
+        <v>838</v>
+      </c>
+      <c r="D961" t="s">
+        <v>842</v>
+      </c>
+      <c r="E961" t="s">
+        <v>785</v>
+      </c>
+      <c r="F961" t="s">
+        <v>838</v>
+      </c>
+      <c r="G961" t="s">
+        <v>842</v>
+      </c>
+      <c r="H961">
+        <v>1389</v>
+      </c>
+      <c r="I961">
+        <v>0</v>
+      </c>
+      <c r="J961">
+        <v>0</v>
+      </c>
+      <c r="K961">
+        <v>0</v>
+      </c>
+      <c r="L961">
+        <v>0</v>
+      </c>
+      <c r="M961" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="962" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A962" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B962" t="s">
+        <v>785</v>
+      </c>
+      <c r="C962" t="s">
+        <v>838</v>
+      </c>
+      <c r="D962" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E962" t="s">
+        <v>785</v>
+      </c>
+      <c r="F962" t="s">
+        <v>838</v>
+      </c>
+      <c r="G962" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H962">
+        <v>1390</v>
+      </c>
+      <c r="I962">
+        <v>0</v>
+      </c>
+      <c r="J962">
+        <v>0</v>
+      </c>
+      <c r="K962">
+        <v>0</v>
+      </c>
+      <c r="L962">
+        <v>0</v>
+      </c>
+      <c r="M962" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="963" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A963" t="s">
+        <v>856</v>
+      </c>
+      <c r="B963" t="s">
+        <v>785</v>
+      </c>
+      <c r="C963" t="s">
+        <v>849</v>
+      </c>
+      <c r="D963" t="s">
+        <v>849</v>
+      </c>
+      <c r="E963" t="s">
+        <v>785</v>
+      </c>
+      <c r="F963" t="s">
+        <v>849</v>
+      </c>
+      <c r="G963" t="s">
+        <v>849</v>
+      </c>
+      <c r="H963">
+        <v>1391</v>
+      </c>
+      <c r="I963">
+        <v>0</v>
+      </c>
+      <c r="J963">
+        <v>0</v>
+      </c>
+      <c r="K963">
+        <v>0</v>
+      </c>
+      <c r="L963">
+        <v>0</v>
+      </c>
+      <c r="M963" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="964" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A964" t="s">
+        <v>808</v>
+      </c>
+      <c r="B964" t="s">
+        <v>785</v>
+      </c>
+      <c r="C964" t="s">
+        <v>801</v>
+      </c>
+      <c r="D964" t="s">
+        <v>809</v>
+      </c>
+      <c r="E964" t="s">
+        <v>785</v>
+      </c>
+      <c r="F964" t="s">
+        <v>801</v>
+      </c>
+      <c r="G964" t="s">
+        <v>809</v>
+      </c>
+      <c r="H964">
+        <v>1392</v>
+      </c>
+      <c r="I964">
+        <v>0</v>
+      </c>
+      <c r="J964">
+        <v>0</v>
+      </c>
+      <c r="K964">
+        <v>0</v>
+      </c>
+      <c r="L964">
+        <v>0</v>
+      </c>
+      <c r="M964" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="965" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A965" t="s">
+        <v>803</v>
+      </c>
+      <c r="B965" t="s">
+        <v>785</v>
+      </c>
+      <c r="C965" t="s">
+        <v>801</v>
+      </c>
+      <c r="D965" t="s">
+        <v>804</v>
+      </c>
+      <c r="E965" t="s">
+        <v>785</v>
+      </c>
+      <c r="F965" t="s">
+        <v>801</v>
+      </c>
+      <c r="G965" t="s">
+        <v>805</v>
+      </c>
+      <c r="H965">
+        <v>1393</v>
+      </c>
+      <c r="I965">
+        <v>0</v>
+      </c>
+      <c r="J965">
+        <v>0</v>
+      </c>
+      <c r="K965">
+        <v>6.6666666666666763E-2</v>
+      </c>
+      <c r="L965">
+        <v>6.6666666666666763E-2</v>
+      </c>
+      <c r="M965" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="966" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A966" t="s">
+        <v>815</v>
+      </c>
+      <c r="B966" t="s">
+        <v>785</v>
+      </c>
+      <c r="C966" t="s">
+        <v>801</v>
+      </c>
+      <c r="D966" t="s">
+        <v>816</v>
+      </c>
+      <c r="E966" t="s">
+        <v>785</v>
+      </c>
+      <c r="F966" t="s">
+        <v>801</v>
+      </c>
+      <c r="G966" t="s">
+        <v>816</v>
+      </c>
+      <c r="H966">
+        <v>1394</v>
+      </c>
+      <c r="I966">
+        <v>0</v>
+      </c>
+      <c r="J966">
+        <v>0</v>
+      </c>
+      <c r="K966">
+        <v>0</v>
+      </c>
+      <c r="L966">
+        <v>0</v>
+      </c>
+      <c r="M966" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="967" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A967" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B967" t="s">
+        <v>221</v>
+      </c>
+      <c r="C967" t="s">
+        <v>287</v>
+      </c>
+      <c r="D967" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E967" t="s">
+        <v>221</v>
+      </c>
+      <c r="F967" t="s">
+        <v>287</v>
+      </c>
+      <c r="G967" t="s">
+        <v>1277</v>
+      </c>
+      <c r="H967">
+        <v>1403</v>
+      </c>
+      <c r="I967">
+        <v>0</v>
+      </c>
+      <c r="J967">
+        <v>0</v>
+      </c>
+      <c r="K967">
+        <v>0</v>
+      </c>
+      <c r="L967">
+        <v>0</v>
+      </c>
+      <c r="M967" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="968" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A968" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B968" t="s">
+        <v>221</v>
+      </c>
+      <c r="C968" t="s">
+        <v>287</v>
+      </c>
+      <c r="D968" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E968" t="s">
+        <v>221</v>
+      </c>
+      <c r="F968" t="s">
+        <v>287</v>
+      </c>
+      <c r="G968" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H968">
+        <v>1404</v>
+      </c>
+      <c r="I968">
+        <v>0</v>
+      </c>
+      <c r="J968">
+        <v>0</v>
+      </c>
+      <c r="K968">
+        <v>0</v>
+      </c>
+      <c r="L968">
+        <v>0</v>
+      </c>
+      <c r="M968" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="969" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A969" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B969" t="s">
+        <v>221</v>
+      </c>
+      <c r="C969" t="s">
+        <v>292</v>
+      </c>
+      <c r="D969" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E969" t="s">
+        <v>221</v>
+      </c>
+      <c r="F969" t="s">
+        <v>292</v>
+      </c>
+      <c r="G969" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H969">
+        <v>1405</v>
+      </c>
+      <c r="I969">
+        <v>0</v>
+      </c>
+      <c r="J969">
+        <v>0</v>
+      </c>
+      <c r="K969">
+        <v>0</v>
+      </c>
+      <c r="L969">
+        <v>0</v>
+      </c>
+      <c r="M969" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="970" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A970" t="s">
+        <v>291</v>
+      </c>
+      <c r="B970" t="s">
+        <v>221</v>
+      </c>
+      <c r="C970" t="s">
+        <v>292</v>
+      </c>
+      <c r="D970" t="s">
+        <v>293</v>
+      </c>
+      <c r="E970" t="s">
+        <v>221</v>
+      </c>
+      <c r="F970" t="s">
+        <v>292</v>
+      </c>
+      <c r="G970" t="s">
+        <v>293</v>
+      </c>
+      <c r="H970">
+        <v>1406</v>
+      </c>
+      <c r="I970">
+        <v>0</v>
+      </c>
+      <c r="J970">
+        <v>0</v>
+      </c>
+      <c r="K970">
+        <v>0</v>
+      </c>
+      <c r="L970">
+        <v>0</v>
+      </c>
+      <c r="M970" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="971" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A971" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B971" t="s">
+        <v>221</v>
+      </c>
+      <c r="C971" t="s">
+        <v>287</v>
+      </c>
+      <c r="D971" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E971" t="s">
+        <v>221</v>
+      </c>
+      <c r="F971" t="s">
+        <v>287</v>
+      </c>
+      <c r="G971" t="s">
+        <v>1282</v>
+      </c>
+      <c r="H971">
+        <v>1407</v>
+      </c>
+      <c r="I971">
+        <v>0</v>
+      </c>
+      <c r="J971">
+        <v>0</v>
+      </c>
+      <c r="K971">
+        <v>0.35714285714285721</v>
+      </c>
+      <c r="L971">
+        <v>0.35714285714285721</v>
+      </c>
+      <c r="M971" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="972" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A972" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B972" t="s">
+        <v>475</v>
+      </c>
+      <c r="C972" t="s">
+        <v>476</v>
+      </c>
+      <c r="D972" t="s">
+        <v>464</v>
+      </c>
+      <c r="E972" t="s">
+        <v>475</v>
+      </c>
+      <c r="F972" t="s">
+        <v>476</v>
+      </c>
+      <c r="G972" t="s">
+        <v>464</v>
+      </c>
+      <c r="H972">
+        <v>1408</v>
+      </c>
+      <c r="I972">
+        <v>0</v>
+      </c>
+      <c r="J972">
+        <v>0</v>
+      </c>
+      <c r="K972">
+        <v>0</v>
+      </c>
+      <c r="L972">
+        <v>0</v>
+      </c>
+      <c r="M972" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="973" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A973" t="s">
+        <v>889</v>
+      </c>
+      <c r="B973" t="s">
+        <v>865</v>
+      </c>
+      <c r="C973" t="s">
+        <v>865</v>
+      </c>
+      <c r="D973" t="s">
+        <v>865</v>
+      </c>
+      <c r="E973" t="s">
+        <v>865</v>
+      </c>
+      <c r="F973" t="s">
+        <v>865</v>
+      </c>
+      <c r="G973" t="s">
+        <v>865</v>
+      </c>
+      <c r="H973">
+        <v>1409</v>
+      </c>
+      <c r="I973">
+        <v>0</v>
+      </c>
+      <c r="J973">
+        <v>0</v>
+      </c>
+      <c r="K973">
+        <v>0</v>
+      </c>
+      <c r="L973">
+        <v>0</v>
+      </c>
+      <c r="M973" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="974" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A974" t="s">
+        <v>495</v>
+      </c>
+      <c r="B974" t="s">
+        <v>475</v>
+      </c>
+      <c r="C974" t="s">
+        <v>493</v>
+      </c>
+      <c r="D974" t="s">
+        <v>496</v>
+      </c>
+      <c r="E974" t="s">
+        <v>475</v>
+      </c>
+      <c r="F974" t="s">
+        <v>493</v>
+      </c>
+      <c r="G974" t="s">
+        <v>496</v>
+      </c>
+      <c r="H974">
+        <v>1410</v>
+      </c>
+      <c r="I974">
+        <v>0</v>
+      </c>
+      <c r="J974">
+        <v>0</v>
+      </c>
+      <c r="K974">
+        <v>0</v>
+      </c>
+      <c r="L974">
+        <v>0</v>
+      </c>
+      <c r="M974" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="975" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A975" t="s">
+        <v>506</v>
+      </c>
+      <c r="B975" t="s">
+        <v>475</v>
+      </c>
+      <c r="C975" t="s">
+        <v>501</v>
+      </c>
+      <c r="D975" t="s">
+        <v>507</v>
+      </c>
+      <c r="E975" t="s">
+        <v>475</v>
+      </c>
+      <c r="F975" t="s">
+        <v>501</v>
+      </c>
+      <c r="G975" t="s">
+        <v>507</v>
+      </c>
+      <c r="H975">
+        <v>1411</v>
+      </c>
+      <c r="I975">
+        <v>0</v>
+      </c>
+      <c r="J975">
+        <v>0</v>
+      </c>
+      <c r="K975">
+        <v>0</v>
+      </c>
+      <c r="L975">
+        <v>0</v>
+      </c>
+      <c r="M975" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="976" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A976" t="s">
+        <v>877</v>
+      </c>
+      <c r="B976" t="s">
+        <v>865</v>
+      </c>
+      <c r="C976" t="s">
+        <v>865</v>
+      </c>
+      <c r="D976" t="s">
+        <v>878</v>
+      </c>
+      <c r="E976" t="s">
+        <v>865</v>
+      </c>
+      <c r="F976" t="s">
+        <v>865</v>
+      </c>
+      <c r="G976" t="s">
+        <v>878</v>
+      </c>
+      <c r="H976">
+        <v>1412</v>
+      </c>
+      <c r="I976">
+        <v>0</v>
+      </c>
+      <c r="J976">
+        <v>0</v>
+      </c>
+      <c r="K976">
+        <v>0</v>
+      </c>
+      <c r="L976">
+        <v>0</v>
+      </c>
+      <c r="M976" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="977" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A977" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B977" t="s">
+        <v>785</v>
+      </c>
+      <c r="C977" t="s">
+        <v>785</v>
+      </c>
+      <c r="D977" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E977" t="s">
+        <v>785</v>
+      </c>
+      <c r="F977" t="s">
+        <v>785</v>
+      </c>
+      <c r="G977" t="s">
+        <v>1042</v>
+      </c>
+      <c r="H977">
+        <v>1413</v>
+      </c>
+      <c r="I977">
+        <v>0</v>
+      </c>
+      <c r="J977">
+        <v>0</v>
+      </c>
+      <c r="K977">
+        <v>0.1970588235294117</v>
+      </c>
+      <c r="L977">
+        <v>0.1970588235294117</v>
+      </c>
+      <c r="M977" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="978" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A978" t="s">
+        <v>492</v>
+      </c>
+      <c r="B978" t="s">
+        <v>475</v>
+      </c>
+      <c r="C978" t="s">
+        <v>493</v>
+      </c>
+      <c r="D978" t="s">
+        <v>494</v>
+      </c>
+      <c r="E978" t="s">
+        <v>475</v>
+      </c>
+      <c r="F978" t="s">
+        <v>493</v>
+      </c>
+      <c r="G978" t="s">
+        <v>494</v>
+      </c>
+      <c r="H978">
+        <v>1414</v>
+      </c>
+      <c r="I978">
+        <v>0</v>
+      </c>
+      <c r="J978">
+        <v>0</v>
+      </c>
+      <c r="K978">
+        <v>0</v>
+      </c>
+      <c r="L978">
+        <v>0</v>
+      </c>
+      <c r="M978" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="979" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>887</v>
+      </c>
+      <c r="B979" t="s">
+        <v>865</v>
+      </c>
+      <c r="C979" t="s">
+        <v>865</v>
+      </c>
+      <c r="D979" t="s">
+        <v>888</v>
+      </c>
+      <c r="E979" t="s">
+        <v>865</v>
+      </c>
+      <c r="F979" t="s">
+        <v>865</v>
+      </c>
+      <c r="G979" t="s">
+        <v>888</v>
+      </c>
+      <c r="H979">
+        <v>1415</v>
+      </c>
+      <c r="I979">
+        <v>0</v>
+      </c>
+      <c r="J979">
+        <v>0</v>
+      </c>
+      <c r="K979">
+        <v>0</v>
+      </c>
+      <c r="L979">
+        <v>0</v>
+      </c>
+      <c r="M979" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="980" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B980" t="s">
+        <v>785</v>
+      </c>
+      <c r="C980" t="s">
+        <v>785</v>
+      </c>
+      <c r="D980" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E980" t="s">
+        <v>785</v>
+      </c>
+      <c r="F980" t="s">
+        <v>785</v>
+      </c>
+      <c r="G980" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H980">
+        <v>1416</v>
+      </c>
+      <c r="I980">
+        <v>0</v>
+      </c>
+      <c r="J980">
+        <v>0</v>
+      </c>
+      <c r="K980">
+        <v>0</v>
+      </c>
+      <c r="L980">
+        <v>0</v>
+      </c>
+      <c r="M980" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="981" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B981" t="s">
+        <v>785</v>
+      </c>
+      <c r="C981" t="s">
+        <v>791</v>
+      </c>
+      <c r="D981" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E981" t="s">
+        <v>785</v>
+      </c>
+      <c r="F981" t="s">
+        <v>791</v>
+      </c>
+      <c r="G981" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H981">
+        <v>1417</v>
+      </c>
+      <c r="I981">
+        <v>0</v>
+      </c>
+      <c r="J981">
+        <v>0</v>
+      </c>
+      <c r="K981">
+        <v>0</v>
+      </c>
+      <c r="L981">
+        <v>0</v>
+      </c>
+      <c r="M981" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="982" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B982" t="s">
+        <v>785</v>
+      </c>
+      <c r="C982" t="s">
+        <v>793</v>
+      </c>
+      <c r="D982" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E982" t="s">
+        <v>785</v>
+      </c>
+      <c r="F982" t="s">
+        <v>793</v>
+      </c>
+      <c r="G982" t="s">
+        <v>1285</v>
+      </c>
+      <c r="H982">
+        <v>1418</v>
+      </c>
+      <c r="I982">
+        <v>0</v>
+      </c>
+      <c r="J982">
+        <v>0</v>
+      </c>
+      <c r="K982">
+        <v>0</v>
+      </c>
+      <c r="L982">
+        <v>0</v>
+      </c>
+      <c r="M982" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="983" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>787</v>
+      </c>
+      <c r="B983" t="s">
+        <v>785</v>
+      </c>
+      <c r="C983" t="s">
+        <v>786</v>
+      </c>
+      <c r="D983" t="s">
+        <v>788</v>
+      </c>
+      <c r="E983" t="s">
+        <v>785</v>
+      </c>
+      <c r="F983" t="s">
+        <v>786</v>
+      </c>
+      <c r="G983" t="s">
+        <v>788</v>
+      </c>
+      <c r="H983">
+        <v>1419</v>
+      </c>
+      <c r="I983">
+        <v>0</v>
+      </c>
+      <c r="J983">
+        <v>0</v>
+      </c>
+      <c r="K983">
+        <v>0</v>
+      </c>
+      <c r="L983">
+        <v>0</v>
+      </c>
+      <c r="M983" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="984" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>789</v>
+      </c>
+      <c r="B984" t="s">
+        <v>785</v>
+      </c>
+      <c r="C984" t="s">
+        <v>786</v>
+      </c>
+      <c r="D984" t="s">
+        <v>437</v>
+      </c>
+      <c r="E984" t="s">
+        <v>785</v>
+      </c>
+      <c r="F984" t="s">
+        <v>786</v>
+      </c>
+      <c r="G984" t="s">
+        <v>437</v>
+      </c>
+      <c r="H984">
+        <v>1420</v>
+      </c>
+      <c r="I984">
+        <v>0</v>
+      </c>
+      <c r="J984">
+        <v>0</v>
+      </c>
+      <c r="K984">
+        <v>0</v>
+      </c>
+      <c r="L984">
+        <v>0</v>
+      </c>
+      <c r="M984" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="985" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>820</v>
+      </c>
+      <c r="B985" t="s">
+        <v>785</v>
+      </c>
+      <c r="C985" t="s">
+        <v>818</v>
+      </c>
+      <c r="D985" t="s">
+        <v>821</v>
+      </c>
+      <c r="E985" t="s">
+        <v>785</v>
+      </c>
+      <c r="F985" t="s">
+        <v>818</v>
+      </c>
+      <c r="G985" t="s">
+        <v>821</v>
+      </c>
+      <c r="H985">
+        <v>1421</v>
+      </c>
+      <c r="I985">
+        <v>0</v>
+      </c>
+      <c r="J985">
+        <v>0</v>
+      </c>
+      <c r="K985">
+        <v>0</v>
+      </c>
+      <c r="L985">
+        <v>0</v>
+      </c>
+      <c r="M985" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="986" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B986" t="s">
+        <v>785</v>
+      </c>
+      <c r="C986" t="s">
+        <v>818</v>
+      </c>
+      <c r="D986" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E986" t="s">
+        <v>785</v>
+      </c>
+      <c r="F986" t="s">
+        <v>818</v>
+      </c>
+      <c r="G986" t="s">
+        <v>1149</v>
+      </c>
+      <c r="H986">
+        <v>1422</v>
+      </c>
+      <c r="I986">
+        <v>0</v>
+      </c>
+      <c r="J986">
+        <v>0</v>
+      </c>
+      <c r="K986">
+        <v>0</v>
+      </c>
+      <c r="L986">
+        <v>0</v>
+      </c>
+      <c r="M986" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="987" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>822</v>
+      </c>
+      <c r="B987" t="s">
+        <v>785</v>
+      </c>
+      <c r="C987" t="s">
+        <v>818</v>
+      </c>
+      <c r="D987" t="s">
+        <v>823</v>
+      </c>
+      <c r="E987" t="s">
+        <v>785</v>
+      </c>
+      <c r="F987" t="s">
+        <v>818</v>
+      </c>
+      <c r="G987" t="s">
+        <v>823</v>
+      </c>
+      <c r="H987">
+        <v>1423</v>
+      </c>
+      <c r="I987">
+        <v>0</v>
+      </c>
+      <c r="J987">
+        <v>0</v>
+      </c>
+      <c r="K987">
+        <v>0</v>
+      </c>
+      <c r="L987">
+        <v>0</v>
+      </c>
+      <c r="M987" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="988" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>862</v>
+      </c>
+      <c r="B988" t="s">
+        <v>785</v>
+      </c>
+      <c r="C988" t="s">
+        <v>861</v>
+      </c>
+      <c r="D988" t="s">
+        <v>863</v>
+      </c>
+      <c r="E988" t="s">
+        <v>785</v>
+      </c>
+      <c r="F988" t="s">
+        <v>861</v>
+      </c>
+      <c r="G988" t="s">
+        <v>863</v>
+      </c>
+      <c r="H988">
+        <v>1424</v>
+      </c>
+      <c r="I988">
+        <v>0</v>
+      </c>
+      <c r="J988">
+        <v>0</v>
+      </c>
+      <c r="K988">
+        <v>0</v>
+      </c>
+      <c r="L988">
+        <v>0</v>
+      </c>
+      <c r="M988" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="989" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>803</v>
+      </c>
+      <c r="B989" t="s">
+        <v>785</v>
+      </c>
+      <c r="C989" t="s">
+        <v>801</v>
+      </c>
+      <c r="D989" t="s">
+        <v>804</v>
+      </c>
+      <c r="E989" t="s">
+        <v>785</v>
+      </c>
+      <c r="F989" t="s">
+        <v>801</v>
+      </c>
+      <c r="G989" t="s">
+        <v>805</v>
+      </c>
+      <c r="H989">
+        <v>1427</v>
+      </c>
+      <c r="I989">
+        <v>0</v>
+      </c>
+      <c r="J989">
+        <v>0</v>
+      </c>
+      <c r="K989">
+        <v>6.6666666666666763E-2</v>
+      </c>
+      <c r="L989">
+        <v>6.6666666666666763E-2</v>
+      </c>
+      <c r="M989" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="990" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B990" t="s">
+        <v>585</v>
+      </c>
+      <c r="C990" t="s">
+        <v>586</v>
+      </c>
+      <c r="D990" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E990" t="s">
+        <v>585</v>
+      </c>
+      <c r="F990" t="s">
+        <v>586</v>
+      </c>
+      <c r="G990" t="s">
+        <v>1237</v>
+      </c>
+      <c r="H990">
+        <v>1428</v>
+      </c>
+      <c r="I990">
+        <v>0</v>
+      </c>
+      <c r="J990">
+        <v>0</v>
+      </c>
+      <c r="K990">
+        <v>0</v>
+      </c>
+      <c r="L990">
+        <v>0</v>
+      </c>
+      <c r="M990" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="991" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>862</v>
+      </c>
+      <c r="B991" t="s">
+        <v>785</v>
+      </c>
+      <c r="C991" t="s">
+        <v>861</v>
+      </c>
+      <c r="D991" t="s">
+        <v>863</v>
+      </c>
+      <c r="E991" t="s">
+        <v>785</v>
+      </c>
+      <c r="F991" t="s">
+        <v>861</v>
+      </c>
+      <c r="G991" t="s">
+        <v>863</v>
+      </c>
+      <c r="H991">
+        <v>1429</v>
+      </c>
+      <c r="I991">
+        <v>0</v>
+      </c>
+      <c r="J991">
+        <v>0</v>
+      </c>
+      <c r="K991">
+        <v>0</v>
+      </c>
+      <c r="L991">
+        <v>0</v>
+      </c>
+      <c r="M991" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="992" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
+        <v>343</v>
+      </c>
+      <c r="B992" t="s">
+        <v>317</v>
+      </c>
+      <c r="C992" t="s">
+        <v>342</v>
+      </c>
+      <c r="D992" t="s">
+        <v>344</v>
+      </c>
+      <c r="E992" t="s">
+        <v>317</v>
+      </c>
+      <c r="F992" t="s">
+        <v>342</v>
+      </c>
+      <c r="G992" t="s">
+        <v>344</v>
+      </c>
+      <c r="H992">
+        <v>1431</v>
+      </c>
+      <c r="I992">
+        <v>0</v>
+      </c>
+      <c r="J992">
+        <v>0</v>
+      </c>
+      <c r="K992">
+        <v>0</v>
+      </c>
+      <c r="L992">
+        <v>0</v>
+      </c>
+      <c r="M992" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="993" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A993" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B993" t="s">
+        <v>317</v>
+      </c>
+      <c r="C993" t="s">
+        <v>342</v>
+      </c>
+      <c r="D993" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E993" t="s">
+        <v>317</v>
+      </c>
+      <c r="F993" t="s">
+        <v>342</v>
+      </c>
+      <c r="G993" t="s">
+        <v>1287</v>
+      </c>
+      <c r="H993">
+        <v>1432</v>
+      </c>
+      <c r="I993">
+        <v>0</v>
+      </c>
+      <c r="J993">
+        <v>0</v>
+      </c>
+      <c r="K993">
+        <v>0</v>
+      </c>
+      <c r="L993">
+        <v>0</v>
+      </c>
+      <c r="M993" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="994" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A994" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B994" t="s">
+        <v>785</v>
+      </c>
+      <c r="C994" t="s">
+        <v>785</v>
+      </c>
+      <c r="D994" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E994" t="s">
+        <v>785</v>
+      </c>
+      <c r="F994" t="s">
+        <v>785</v>
+      </c>
+      <c r="G994" t="s">
+        <v>1289</v>
+      </c>
+      <c r="H994">
+        <v>1433</v>
+      </c>
+      <c r="I994">
+        <v>0</v>
+      </c>
+      <c r="J994">
+        <v>0</v>
+      </c>
+      <c r="K994">
+        <v>0</v>
+      </c>
+      <c r="L994">
+        <v>0</v>
+      </c>
+      <c r="M994" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="995" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A995" t="s">
+        <v>811</v>
+      </c>
+      <c r="B995" t="s">
+        <v>785</v>
+      </c>
+      <c r="C995" t="s">
+        <v>801</v>
+      </c>
+      <c r="D995" t="s">
+        <v>812</v>
+      </c>
+      <c r="E995" t="s">
+        <v>785</v>
+      </c>
+      <c r="F995" t="s">
+        <v>801</v>
+      </c>
+      <c r="G995" t="s">
+        <v>812</v>
+      </c>
+      <c r="H995">
+        <v>1434</v>
+      </c>
+      <c r="I995">
+        <v>0</v>
+      </c>
+      <c r="J995">
+        <v>0</v>
+      </c>
+      <c r="K995">
+        <v>0</v>
+      </c>
+      <c r="L995">
+        <v>0</v>
+      </c>
+      <c r="M995" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="996" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A996" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B996" t="s">
+        <v>785</v>
+      </c>
+      <c r="C996" t="s">
+        <v>785</v>
+      </c>
+      <c r="D996" t="s">
+        <v>810</v>
+      </c>
+      <c r="E996" t="s">
+        <v>785</v>
+      </c>
+      <c r="F996" t="s">
+        <v>785</v>
+      </c>
+      <c r="G996" t="s">
+        <v>810</v>
+      </c>
+      <c r="H996">
+        <v>1435</v>
+      </c>
+      <c r="I996">
+        <v>0</v>
+      </c>
+      <c r="J996">
+        <v>0</v>
+      </c>
+      <c r="K996">
+        <v>0</v>
+      </c>
+      <c r="L996">
+        <v>0</v>
+      </c>
+      <c r="M996" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="997" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B997" t="s">
+        <v>785</v>
+      </c>
+      <c r="C997" t="s">
+        <v>849</v>
+      </c>
+      <c r="D997" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E997" t="s">
+        <v>785</v>
+      </c>
+      <c r="F997" t="s">
+        <v>849</v>
+      </c>
+      <c r="G997" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H997">
+        <v>1436</v>
+      </c>
+      <c r="I997">
+        <v>0</v>
+      </c>
+      <c r="J997">
+        <v>0</v>
+      </c>
+      <c r="K997">
+        <v>0</v>
+      </c>
+      <c r="L997">
+        <v>0</v>
+      </c>
+      <c r="M997" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="998" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
+        <v>851</v>
+      </c>
+      <c r="B998" t="s">
+        <v>785</v>
+      </c>
+      <c r="C998" t="s">
+        <v>849</v>
+      </c>
+      <c r="D998" t="s">
+        <v>852</v>
+      </c>
+      <c r="E998" t="s">
+        <v>785</v>
+      </c>
+      <c r="F998" t="s">
+        <v>849</v>
+      </c>
+      <c r="G998" t="s">
+        <v>852</v>
+      </c>
+      <c r="H998">
+        <v>1437</v>
+      </c>
+      <c r="I998">
+        <v>0</v>
+      </c>
+      <c r="J998">
+        <v>0</v>
+      </c>
+      <c r="K998">
+        <v>0</v>
+      </c>
+      <c r="L998">
+        <v>0</v>
+      </c>
+      <c r="M998" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="999" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A999" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B999" t="s">
+        <v>785</v>
+      </c>
+      <c r="C999" t="s">
+        <v>861</v>
+      </c>
+      <c r="D999" t="s">
+        <v>861</v>
+      </c>
+      <c r="E999" t="s">
+        <v>785</v>
+      </c>
+      <c r="F999" t="s">
+        <v>861</v>
+      </c>
+      <c r="G999" t="s">
+        <v>861</v>
+      </c>
+      <c r="H999">
+        <v>1438</v>
+      </c>
+      <c r="I999">
+        <v>0</v>
+      </c>
+      <c r="J999">
+        <v>0</v>
+      </c>
+      <c r="K999">
+        <v>0</v>
+      </c>
+      <c r="L999">
+        <v>0</v>
+      </c>
+      <c r="M999" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1000" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>785</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>838</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>785</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>838</v>
+      </c>
+      <c r="G1000" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H1000">
+        <v>1439</v>
+      </c>
+      <c r="I1000">
+        <v>0</v>
+      </c>
+      <c r="J1000">
+        <v>0</v>
+      </c>
+      <c r="K1000">
+        <v>4.4444444444444509E-2</v>
+      </c>
+      <c r="L1000">
+        <v>4.4444444444444509E-2</v>
+      </c>
+      <c r="M1000" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1001" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1001" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1001">
+        <v>1440</v>
+      </c>
+      <c r="I1001">
+        <v>0</v>
+      </c>
+      <c r="J1001">
+        <v>0</v>
+      </c>
+      <c r="K1001">
+        <v>0</v>
+      </c>
+      <c r="L1001">
+        <v>0</v>
+      </c>
+      <c r="M1001" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1002" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1002" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1002">
+        <v>1441</v>
+      </c>
+      <c r="I1002">
+        <v>0</v>
+      </c>
+      <c r="J1002">
+        <v>0</v>
+      </c>
+      <c r="K1002">
+        <v>0</v>
+      </c>
+      <c r="L1002">
+        <v>0</v>
+      </c>
+      <c r="M1002" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1003" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1003">
+        <v>1442</v>
+      </c>
+      <c r="I1003">
+        <v>0</v>
+      </c>
+      <c r="J1003">
+        <v>0</v>
+      </c>
+      <c r="K1003">
+        <v>0</v>
+      </c>
+      <c r="L1003">
+        <v>0</v>
+      </c>
+      <c r="M1003" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1004" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1004" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1004">
+        <v>1443</v>
+      </c>
+      <c r="I1004">
+        <v>0</v>
+      </c>
+      <c r="J1004">
+        <v>0</v>
+      </c>
+      <c r="K1004">
+        <v>0</v>
+      </c>
+      <c r="L1004">
+        <v>0</v>
+      </c>
+      <c r="M1004" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1005" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1005" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1005">
+        <v>1444</v>
+      </c>
+      <c r="I1005">
+        <v>0</v>
+      </c>
+      <c r="J1005">
+        <v>0</v>
+      </c>
+      <c r="K1005">
+        <v>0</v>
+      </c>
+      <c r="L1005">
+        <v>0</v>
+      </c>
+      <c r="M1005" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1006" t="s">
+        <v>970</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>971</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>317</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>337</v>
+      </c>
+      <c r="G1006" t="s">
+        <v>971</v>
+      </c>
+      <c r="H1006">
+        <v>1447</v>
+      </c>
+      <c r="I1006">
+        <v>0</v>
+      </c>
+      <c r="J1006">
+        <v>0</v>
+      </c>
+      <c r="K1006">
+        <v>0</v>
+      </c>
+      <c r="L1006">
+        <v>0</v>
+      </c>
+      <c r="M1006" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1007" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1007" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1007">
+        <v>1449</v>
+      </c>
+      <c r="I1007">
+        <v>0</v>
+      </c>
+      <c r="J1007">
+        <v>0</v>
+      </c>
+      <c r="K1007">
+        <v>0</v>
+      </c>
+      <c r="L1007">
+        <v>0</v>
+      </c>
+      <c r="M1007" t="s">
+        <v>932</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M921" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M989" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>